<commit_message>
jin : flask source update
</commit_message>
<xml_diff>
--- a/source/11_Flask/data/ex3_xlwing.xlsx
+++ b/source/11_Flask/data/ex3_xlwing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/mbc/ai_x/source/12_Flask/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ai_x\source\11_flask\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F7E0A38-0849-C34D-9D25-6B730FCD7BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B348AB7-B94D-4CA5-AA89-F2D65C19ADAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="10000" windowHeight="5800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13836" yWindow="1452" windowWidth="15660" windowHeight="9348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,17 +381,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="5" max="5" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -405,7 +405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>2010</v>
       </c>
@@ -419,7 +419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2012</v>
       </c>
@@ -433,7 +433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2024</v>
       </c>

</xml_diff>